<commit_message>
BÀN GIAO SOURCE CODE CHO ANH TÙNG
</commit_message>
<xml_diff>
--- a/CREADMENU.xlsx
+++ b/CREADMENU.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>mnuTo</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>[TO]</t>
+  </si>
+  <si>
+    <t>LOAI_HD</t>
+  </si>
+  <si>
+    <t>Loại hợp đồng</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,8 +401,9 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="115.5703125" customWidth="1"/>
+    <col min="7" max="7" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -444,7 +451,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f t="shared" ref="G2:G3" si="0">" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C2&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'"&amp;C2&amp;"' AS [KEY_MENU],    N'"&amp;D2&amp;"' AS [TEN_MENU] ,    N'"&amp;E2&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E2&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C2&amp;"' END  "</f>
+        <f t="shared" ref="G2:G8" si="0">" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C2&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'"&amp;C2&amp;"' AS [KEY_MENU],    N'"&amp;D2&amp;"' AS [TEN_MENU] ,    N'"&amp;E2&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E2&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C2&amp;"' END  "</f>
         <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuTo' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnuTo' AS [KEY_MENU],    N'Tổ' AS [TEN_MENU] ,    N'Team' AS [TEN_MENU_ANH],      N'Team' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuTo' END  </v>
       </c>
     </row>
@@ -475,9 +482,23 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>spGetList</v>
+        <v>spGetListLOAI_HD</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C6" si="2">"mnu"&amp;A4</f>
+        <v>mnuLOAI_HD</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuLOAI_HD' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnuLOAI_HD' AS [KEY_MENU],    N'Loại hợp đồng' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuLOAI_HD' END  </v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -485,23 +506,47 @@
         <f t="shared" si="1"/>
         <v>spGetList</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="str">
+        <f t="shared" si="2"/>
+        <v>mnu</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f t="shared" si="1"/>
         <v>spGetList</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="str">
+        <f t="shared" si="2"/>
+        <v>mnu</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f t="shared" si="1"/>
         <v>spGetList</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f t="shared" si="1"/>
         <v>spGetList</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ban giao code cho anh tung
</commit_message>
<xml_diff>
--- a/CREADMENU.xlsx
+++ b/CREADMENU.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>mnuTo</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Loại hợp đồng</t>
+  </si>
+  <si>
+    <t>GROUP</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,10 +406,11 @@
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -425,12 +429,15 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="str">
-        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C1&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'"&amp;C1&amp;"' AS [KEY_MENU],    N'"&amp;D1&amp;"' AS [TEN_MENU] ,    N'"&amp;E1&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E1&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C1&amp;"' END  "</f>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'KEY_MENU' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'KEY_MENU' AS [KEY_MENU],    N'TEN_MENU' AS [TEN_MENU] ,    N'TEN_MENU_ANH' AS [TEN_MENU_ANH],      N'TEN_MENU_ANH' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'KEY_MENU' END  </v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C1&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;C1&amp;"' AS [KEY_MENU],    N'"&amp;D1&amp;"' AS [TEN_MENU] ,    N'"&amp;E1&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E1&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;G1&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C1&amp;"' END  "</f>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'KEY_MENU' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'KEY_MENU' AS [KEY_MENU],    N'TEN_MENU' AS [TEN_MENU] ,    N'TEN_MENU_ANH' AS [TEN_MENU_ANH],      N'TEN_MENU_ANH' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'GROUP' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'KEY_MENU' END  </v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -450,17 +457,17 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="str">
-        <f t="shared" ref="G2:G8" si="0">" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C2&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'"&amp;C2&amp;"' AS [KEY_MENU],    N'"&amp;D2&amp;"' AS [TEN_MENU] ,    N'"&amp;E2&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E2&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C2&amp;"' END  "</f>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuTo' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnuTo' AS [KEY_MENU],    N'Tổ' AS [TEN_MENU] ,    N'Team' AS [TEN_MENU_ANH],      N'Team' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuTo' END  </v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="str">
+        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C2&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;C2&amp;"' AS [KEY_MENU],    N'"&amp;D2&amp;"' AS [TEN_MENU] ,    N'"&amp;E2&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E2&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;G2&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C2&amp;"' END  "</f>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuTo' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuTo' AS [KEY_MENU],    N'Tổ' AS [TEN_MENU] ,    N'Team' AS [TEN_MENU_ANH],      N'Team' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuTo' END  </v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B8" si="1">"spGetList"&amp;A3</f>
+        <f t="shared" ref="B3:B8" si="0">"spGetList"&amp;A3</f>
         <v>spGetListCHUC_VU</v>
       </c>
       <c r="C3" t="str">
@@ -476,17 +483,18 @@
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuCHUC_VU' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnuCHUC_VU' AS [KEY_MENU],    N'Chức vụ' AS [TEN_MENU] ,    N'Position' AS [TEN_MENU_ANH],      N'Position' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuCHUC_VU' END  </v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H2:H8" si="1">" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C3&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;C3&amp;"' AS [KEY_MENU],    N'"&amp;D3&amp;"' AS [TEN_MENU] ,    N'"&amp;E3&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E3&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;G3&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C3&amp;"' END  "</f>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuCHUC_VU' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuCHUC_VU' AS [KEY_MENU],    N'Chức vụ' AS [TEN_MENU] ,    N'Position' AS [TEN_MENU_ANH],      N'Position' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuCHUC_VU' END  </v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>spGetListLOAI_HD</v>
       </c>
       <c r="C4" t="str">
@@ -496,57 +504,57 @@
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="H4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuLOAI_HD' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuLOAI_HD' AS [KEY_MENU],    N'Loại hợp đồng' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuLOAI_HD' END  </v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuLOAI_HD' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnuLOAI_HD' AS [KEY_MENU],    N'Loại hợp đồng' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuLOAI_HD' END  </v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
-        <f t="shared" si="1"/>
         <v>spGetList</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="2"/>
         <v>mnu</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="H5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B6" t="str">
-        <f t="shared" si="1"/>
         <v>spGetList</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="2"/>
         <v>mnu</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
+        <v>spGetList</v>
+      </c>
+      <c r="H7" s="1" t="str">
         <f t="shared" si="1"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
         <v>spGetList</v>
       </c>
-      <c r="G7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
+      <c r="H8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>spGetList</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ban giao code cho anh nhat
</commit_message>
<xml_diff>
--- a/CREADMENU.xlsx
+++ b/CREADMENU.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>mnuTo</t>
   </si>
@@ -72,6 +73,15 @@
   </si>
   <si>
     <t>GROUP</t>
+  </si>
+  <si>
+    <t>chú ý</t>
+  </si>
+  <si>
+    <t>XI_NGHIEP</t>
+  </si>
+  <si>
+    <t>Ten User control ( Chu y ham khoi tao fai co ID truyen vao    Int64 iId)</t>
   </si>
 </sst>
 </file>
@@ -393,167 +403,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="50.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="str">
-        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C1&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;C1&amp;"' AS [KEY_MENU],    N'"&amp;D1&amp;"' AS [TEN_MENU] ,    N'"&amp;E1&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E1&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;G1&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C1&amp;"' END  "</f>
+      <c r="I1" s="1" t="str">
+        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;D1&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;D1&amp;"' AS [KEY_MENU],    N'"&amp;E1&amp;"' AS [TEN_MENU] ,    N'"&amp;F1&amp;"' AS [TEN_MENU_ANH],      N'"&amp;F1&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;H1&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;D1&amp;"' END  "</f>
         <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'KEY_MENU' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'KEY_MENU' AS [KEY_MENU],    N'TEN_MENU' AS [TEN_MENU] ,    N'TEN_MENU_ANH' AS [TEN_MENU_ANH],      N'TEN_MENU_ANH' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'GROUP' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'KEY_MENU' END  </v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"ucEdit" &amp; B2</f>
+        <v>ucEdit[TO]</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="str">
-        <f>"spGetList"&amp;A2</f>
+      <c r="C2" t="str">
+        <f>"spGetList"&amp;B2</f>
         <v>spGetList[TO]</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C2&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;C2&amp;"' AS [KEY_MENU],    N'"&amp;D2&amp;"' AS [TEN_MENU] ,    N'"&amp;E2&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E2&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;G2&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C2&amp;"' END  "</f>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;D2&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;D2&amp;"' AS [KEY_MENU],    N'"&amp;E2&amp;"' AS [TEN_MENU] ,    N'"&amp;F2&amp;"' AS [TEN_MENU_ANH],      N'"&amp;F2&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;H2&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;D2&amp;"' END  "</f>
         <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuTo' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuTo' AS [KEY_MENU],    N'Tổ' AS [TEN_MENU] ,    N'Team' AS [TEN_MENU_ANH],      N'Team' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuTo' END  </v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A6" si="0">"ucEdit" &amp; B3</f>
+        <v>ucEditCHUC_VU</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B8" si="0">"spGetList"&amp;A3</f>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C8" si="1">"spGetList"&amp;B3</f>
         <v>spGetListCHUC_VU</v>
       </c>
-      <c r="C3" t="str">
-        <f>"mnu"&amp;A3</f>
+      <c r="D3" t="str">
+        <f>"mnu"&amp;B3</f>
         <v>mnuCHUC_VU</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H2:H8" si="1">" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;C3&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;C3&amp;"' AS [KEY_MENU],    N'"&amp;D3&amp;"' AS [TEN_MENU] ,    N'"&amp;E3&amp;"' AS [TEN_MENU_ANH],      N'"&amp;E3&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;G3&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;C3&amp;"' END  "</f>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I8" si="2">" IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'"&amp;D3&amp;"' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'"&amp;D3&amp;"' AS [KEY_MENU],    N'"&amp;E3&amp;"' AS [TEN_MENU] ,    N'"&amp;F3&amp;"' AS [TEN_MENU_ANH],      N'"&amp;F3&amp;"' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'"&amp;H3&amp;"' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'"&amp;D3&amp;"' END  "</f>
         <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuCHUC_VU' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuCHUC_VU' AS [KEY_MENU],    N'Chức vụ' AS [TEN_MENU] ,    N'Position' AS [TEN_MENU_ANH],      N'Position' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuCHUC_VU' END  </v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>ucEditLOAI_HD</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>spGetListLOAI_HD</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D6" si="3">"mnu"&amp;B4</f>
+        <v>mnuLOAI_HD</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuLOAI_HD' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuLOAI_HD' AS [KEY_MENU],    N'Loại hợp đồng' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuLOAI_HD' END  </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>spGetListLOAI_HD</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C6" si="2">"mnu"&amp;A4</f>
-        <v>mnuLOAI_HD</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="str">
+        <v>ucEditXI_NGHIEP</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuLOAI_HD' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuLOAI_HD' AS [KEY_MENU],    N'Loại hợp đồng' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuLOAI_HD' END  </v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
+        <v>spGetListXI_NGHIEP</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="3"/>
+        <v>mnuXI_NGHIEP</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnuXI_NGHIEP' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnuXI_NGHIEP' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnuXI_NGHIEP' END  </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
+        <v>ucEdit</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
         <v>spGetList</v>
       </c>
-      <c r="C5" t="str">
+      <c r="D6" t="str">
+        <f t="shared" si="3"/>
+        <v>mnu</v>
+      </c>
+      <c r="I6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>mnu</v>
-      </c>
-      <c r="H5" s="1" t="str">
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
         <v>spGetList</v>
       </c>
-      <c r="C6" t="str">
+      <c r="I7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>mnu</v>
-      </c>
-      <c r="H6" s="1" t="str">
+        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'mnu' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'mnu' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'mnu' END  </v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
         <v>spGetList</v>
       </c>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>spGetList</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> IF NOT EXISTS(SELECT * FROM dbo.MENU WHERE [KEY_MENU] =  N'' ) BEGIN INSERT INTO [dbo].[MENU]([KEY_MENU],[TEN_MENU],[TEN_MENU_ANH],[TEN_MENU_HOA],[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],[CONTROLS]) SELECT N'' AS [KEY_MENU],    N'' AS [TEN_MENU] ,    N'' AS [TEN_MENU_ANH],      N'' AS [TEN_MENU_HOA] ,[ROOT],[HIDE],[BACK_COLOR],[IMG],[STT_MENU],    N'' AS [CONTROLS] FROM dbo.MENU WHERE [KEY_MENU] = 'mnuDon_vi'   INSERT INTO dbo.NHOM_MENU (ID_MENU, ID_NHOM )  SELECT TOP 1 ID_MENU ,1 FROM dbo.MENU WHERE KEY_MENU =  N'' END  </v>
       </c>
     </row>
@@ -561,4 +596,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>